<commit_message>
Update of thresholds data
</commit_message>
<xml_diff>
--- a/SpeciesTables/SpeciesThresholds.xlsx
+++ b/SpeciesTables/SpeciesThresholds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/ClimateChange/R_code/TempSynthesis/SpeciesTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763AF2FA-0CB0-471E-8C5E-51B3D89629EC}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678D5F11-35C4-405D-8BE2-C5CE6252CAE6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F95700F2-2543-4D53-85A7-DBBD5FF11025}"/>
+    <workbookView minimized="1" xWindow="1425" yWindow="570" windowWidth="21600" windowHeight="11265" xr2:uid="{F95700F2-2543-4D53-85A7-DBBD5FF11025}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,8 +619,8 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,10 +2053,10 @@
         <v>30</v>
       </c>
       <c r="F55" s="6">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G55" s="6">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Changed some of the thresholds (asian clam and delta smelt)
</commit_message>
<xml_diff>
--- a/SpeciesTables/SpeciesThresholds.xlsx
+++ b/SpeciesTables/SpeciesThresholds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/ClimateChange/R_code/TempSynthesis/SpeciesTables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/WaterTemp/TempSynthesis/SpeciesTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678D5F11-35C4-405D-8BE2-C5CE6252CAE6}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A8CA11B-59A3-4912-9542-880E91A3BC55}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1425" yWindow="570" windowWidth="21600" windowHeight="11265" xr2:uid="{F95700F2-2543-4D53-85A7-DBBD5FF11025}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F95700F2-2543-4D53-85A7-DBBD5FF11025}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="66">
   <si>
     <t>Species</t>
   </si>
@@ -619,8 +619,8 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,10 +825,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3">
         <v>26.5</v>
@@ -1995,16 +1995,16 @@
         <v>31</v>
       </c>
       <c r="D53" s="6">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E53" s="6">
-        <v>23</v>
-      </c>
-      <c r="F53" s="6">
         <v>28</v>
       </c>
-      <c r="G53" s="6">
-        <v>28</v>
+      <c r="F53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>7</v>

</xml_diff>